<commit_message>
use s3 bucket as
</commit_message>
<xml_diff>
--- a/test/resources/AutoCalc_Soccer_EventLog.xlsx
+++ b/test/resources/AutoCalc_Soccer_EventLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="18120" windowHeight="13890"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="18120" windowHeight="13890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EventType" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <author>vetal</author>
   </authors>
   <commentList>
-    <comment ref="A42" authorId="0">
+    <comment ref="A45" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="109">
   <si>
     <t>Half 1</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>AnyString</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Numeric(1,120)</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1053,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1049,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,25 +1273,25 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>70</v>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>19</v>
+        <v>106</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>20</v>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -1287,10 +1299,10 @@
         <v>70</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1298,10 +1310,10 @@
         <v>70</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1312,62 +1324,62 @@
         <v>67</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36" t="s">
+    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C22" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D22" s="36" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+    <row r="23" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D24" s="35" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1375,65 +1387,65 @@
         <v>56</v>
       </c>
       <c r="C25" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="36" t="s">
+      <c r="D26" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C27" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>19</v>
+      <c r="D27" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C30" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>58</v>
+      <c r="D30" s="35" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -1441,65 +1453,65 @@
         <v>40</v>
       </c>
       <c r="C31" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="36" t="s">
+      <c r="D32" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C33" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>19</v>
+      <c r="D33" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C36" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>58</v>
+      <c r="D36" s="35" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,10 +1519,10 @@
         <v>16</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,208 +1533,241 @@
         <v>67</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="36" t="s">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C42" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D42" s="36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="38" t="s">
+    <row r="43" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="38" t="s">
         <v>57</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>7</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>58</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>7</v>
-      </c>
       <c r="B44" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>8</v>
-      </c>
       <c r="B45" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C46" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
       <c r="B47" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>8</v>
+      </c>
       <c r="B48" s="38" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>8</v>
+      </c>
       <c r="B49" s="38" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C49" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="38" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C50" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="38" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C52" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="38" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C53" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="38" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>1</v>
-      </c>
       <c r="B55" s="38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C55" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D55" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1742,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,8 +1825,12 @@
       <c r="G1" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="2"/>
+      <c r="H1" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>105</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>

</xml_diff>